<commit_message>
Chi tiet nhan vien
</commit_message>
<xml_diff>
--- a/Img/demo.xlsx
+++ b/Img/demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D\NAM 3\HKI\PHAT TRIEN UNG DUNG\BTL\BTLPTUD\QuanLiXeMay\Img\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572FF254-21F7-46BE-881F-D283BC8464B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8510CB-A22D-4799-BBE1-2630FE883F32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5364" yWindow="600" windowWidth="14916" windowHeight="10476" xr2:uid="{EB2C2BA9-C14E-48C1-B577-63910D89887D}"/>
+    <workbookView xWindow="2808" yWindow="2028" windowWidth="14796" windowHeight="10476" xr2:uid="{EB2C2BA9-C14E-48C1-B577-63910D89887D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="136">
   <si>
     <t>Mã xe máy</t>
   </si>
@@ -205,6 +205,243 @@
   </si>
   <si>
     <t>M5</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>M8</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>M10</t>
+  </si>
+  <si>
+    <t>M11</t>
+  </si>
+  <si>
+    <t>M12</t>
+  </si>
+  <si>
+    <t>M13</t>
+  </si>
+  <si>
+    <t>M14</t>
+  </si>
+  <si>
+    <t>M15</t>
+  </si>
+  <si>
+    <t>M16</t>
+  </si>
+  <si>
+    <t>M17</t>
+  </si>
+  <si>
+    <t>M18</t>
+  </si>
+  <si>
+    <t>M19</t>
+  </si>
+  <si>
+    <t>M20</t>
+  </si>
+  <si>
+    <t>Xe 6</t>
+  </si>
+  <si>
+    <t>Xe 7</t>
+  </si>
+  <si>
+    <t>Xe 8</t>
+  </si>
+  <si>
+    <t>Xe 9</t>
+  </si>
+  <si>
+    <t>Xe 10</t>
+  </si>
+  <si>
+    <t>Xe 11</t>
+  </si>
+  <si>
+    <t>Xe 12</t>
+  </si>
+  <si>
+    <t>Xe 13</t>
+  </si>
+  <si>
+    <t>Xe 14</t>
+  </si>
+  <si>
+    <t>Xe 15</t>
+  </si>
+  <si>
+    <t>Xe 16</t>
+  </si>
+  <si>
+    <t>Xe 17</t>
+  </si>
+  <si>
+    <t>Xe 18</t>
+  </si>
+  <si>
+    <t>Xe 19</t>
+  </si>
+  <si>
+    <t>Xe 20</t>
+  </si>
+  <si>
+    <t>k6</t>
+  </si>
+  <si>
+    <t>k7</t>
+  </si>
+  <si>
+    <t>k8</t>
+  </si>
+  <si>
+    <t>k9</t>
+  </si>
+  <si>
+    <t>k10</t>
+  </si>
+  <si>
+    <t>k11</t>
+  </si>
+  <si>
+    <t>k12</t>
+  </si>
+  <si>
+    <t>k13</t>
+  </si>
+  <si>
+    <t>k14</t>
+  </si>
+  <si>
+    <t>k15</t>
+  </si>
+  <si>
+    <t>k16</t>
+  </si>
+  <si>
+    <t>k17</t>
+  </si>
+  <si>
+    <t>k18</t>
+  </si>
+  <si>
+    <t>k19</t>
+  </si>
+  <si>
+    <t>k20</t>
+  </si>
+  <si>
+    <t>s6</t>
+  </si>
+  <si>
+    <t>s7</t>
+  </si>
+  <si>
+    <t>s8</t>
+  </si>
+  <si>
+    <t>s9</t>
+  </si>
+  <si>
+    <t>s10</t>
+  </si>
+  <si>
+    <t>s11</t>
+  </si>
+  <si>
+    <t>s12</t>
+  </si>
+  <si>
+    <t>s13</t>
+  </si>
+  <si>
+    <t>s14</t>
+  </si>
+  <si>
+    <t>s15</t>
+  </si>
+  <si>
+    <t>s16</t>
+  </si>
+  <si>
+    <t>s17</t>
+  </si>
+  <si>
+    <t>s18</t>
+  </si>
+  <si>
+    <t>s19</t>
+  </si>
+  <si>
+    <t>s20</t>
+  </si>
+  <si>
+    <t>Hãng xe</t>
+  </si>
+  <si>
+    <t>Sirius</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>SZK1</t>
+  </si>
+  <si>
+    <t>KW1</t>
+  </si>
+  <si>
+    <t>SZK2</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>KW2</t>
+  </si>
+  <si>
+    <t>SZK3</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>KW3</t>
+  </si>
+  <si>
+    <t>SZK4</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>KW4</t>
+  </si>
+  <si>
+    <t>M21</t>
+  </si>
+  <si>
+    <t>Xe 21</t>
+  </si>
+  <si>
+    <t>k21</t>
+  </si>
+  <si>
+    <t>s21</t>
   </si>
 </sst>
 </file>
@@ -562,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51282798-F2B0-43F9-976F-8297718698E0}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,11 +810,11 @@
     <col min="1" max="1" width="14.21875" customWidth="1"/>
     <col min="2" max="2" width="11.109375" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" customWidth="1"/>
-    <col min="13" max="13" width="11.77734375" customWidth="1"/>
-    <col min="14" max="14" width="34.5546875" customWidth="1"/>
+    <col min="14" max="14" width="11.77734375" customWidth="1"/>
+    <col min="15" max="15" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -612,16 +849,19 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -659,13 +899,16 @@
         <v>37</v>
       </c>
       <c r="M2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" t="s">
         <v>42</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -673,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -703,13 +946,16 @@
         <v>38</v>
       </c>
       <c r="M3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N3" t="s">
         <v>43</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -717,7 +963,7 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -747,13 +993,16 @@
         <v>39</v>
       </c>
       <c r="M4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N4" t="s">
         <v>44</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -761,7 +1010,7 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -791,13 +1040,16 @@
         <v>40</v>
       </c>
       <c r="M5" t="s">
+        <v>120</v>
+      </c>
+      <c r="N5" t="s">
         <v>45</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -805,7 +1057,7 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -835,10 +1087,765 @@
         <v>41</v>
       </c>
       <c r="M6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" t="s">
         <v>46</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" t="s">
+        <v>118</v>
+      </c>
+      <c r="N7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8">
+        <v>110</v>
+      </c>
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N8" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9">
+        <v>125</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" t="s">
+        <v>123</v>
+      </c>
+      <c r="N9" t="s">
+        <v>44</v>
+      </c>
+      <c r="O9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10">
+        <v>150</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" t="s">
+        <v>124</v>
+      </c>
+      <c r="N10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" t="s">
+        <v>106</v>
+      </c>
+      <c r="I11">
+        <v>175</v>
+      </c>
+      <c r="J11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" t="s">
+        <v>125</v>
+      </c>
+      <c r="N11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12">
+        <v>50</v>
+      </c>
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" t="s">
+        <v>118</v>
+      </c>
+      <c r="N12" t="s">
+        <v>42</v>
+      </c>
+      <c r="O12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13">
+        <v>110</v>
+      </c>
+      <c r="J13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" t="s">
+        <v>119</v>
+      </c>
+      <c r="N13" t="s">
+        <v>43</v>
+      </c>
+      <c r="O13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>26</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14">
+        <v>125</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" t="s">
+        <v>126</v>
+      </c>
+      <c r="N14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>28</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15">
+        <v>150</v>
+      </c>
+      <c r="J15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N15" t="s">
+        <v>45</v>
+      </c>
+      <c r="O15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <v>25</v>
+      </c>
+      <c r="F16">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16">
+        <v>175</v>
+      </c>
+      <c r="J16" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" t="s">
+        <v>128</v>
+      </c>
+      <c r="N16" t="s">
+        <v>46</v>
+      </c>
+      <c r="O16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>32</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17">
+        <v>50</v>
+      </c>
+      <c r="J17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" t="s">
+        <v>118</v>
+      </c>
+      <c r="N17" t="s">
+        <v>42</v>
+      </c>
+      <c r="O17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>34</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18">
+        <v>110</v>
+      </c>
+      <c r="J18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" t="s">
+        <v>119</v>
+      </c>
+      <c r="N18" t="s">
+        <v>43</v>
+      </c>
+      <c r="O18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>36</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>36</v>
+      </c>
+      <c r="G19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" t="s">
+        <v>114</v>
+      </c>
+      <c r="I19">
+        <v>125</v>
+      </c>
+      <c r="J19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" t="s">
+        <v>39</v>
+      </c>
+      <c r="M19" t="s">
+        <v>129</v>
+      </c>
+      <c r="N19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>38</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>36</v>
+      </c>
+      <c r="G20" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20">
+        <v>150</v>
+      </c>
+      <c r="J20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" t="s">
+        <v>130</v>
+      </c>
+      <c r="N20" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>40</v>
+      </c>
+      <c r="E21">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <v>36</v>
+      </c>
+      <c r="G21" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21">
+        <v>175</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" t="s">
+        <v>36</v>
+      </c>
+      <c r="L21" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" t="s">
+        <v>131</v>
+      </c>
+      <c r="N21" t="s">
+        <v>46</v>
+      </c>
+      <c r="O21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <v>25</v>
+      </c>
+      <c r="F22">
+        <v>36</v>
+      </c>
+      <c r="G22" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" t="s">
+        <v>135</v>
+      </c>
+      <c r="I22">
+        <v>175</v>
+      </c>
+      <c r="J22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22">
+        <v>21</v>
+      </c>
+      <c r="L22">
+        <v>21</v>
+      </c>
+      <c r="M22">
+        <v>21</v>
+      </c>
+      <c r="N22">
+        <v>21</v>
+      </c>
+      <c r="O22">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>